<commit_message>
Worked on group PLS
</commit_message>
<xml_diff>
--- a/Biomarker_annotation.xlsx
+++ b/Biomarker_annotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luischavesrodriguez/OneDrive - Imperial College London/MScHDA/Term2/TDS/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catri\OneDrive\Documents\MSc HDA\Translational Data Sciences\BEES_TDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{9A24B856-B701-2743-ADFC-7E0A35D99268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9CD5D471-0A13-FE4A-BE86-2FDB23157BC3}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{9A24B856-B701-2743-ADFC-7E0A35D99268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7D89798-0B7E-4087-9888-7BB72877E340}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{85285DCB-5536-7D41-BDF8-0554B552EAE8}"/>
+    <workbookView xWindow="10490" yWindow="0" windowWidth="7500" windowHeight="10200" xr2:uid="{85285DCB-5536-7D41-BDF8-0554B552EAE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,11 +538,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06EC7B42-54D3-D849-9328-5C0F1D16A97A}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
@@ -552,7 +552,7 @@
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -572,7 +572,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>30620</v>
       </c>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>30600</v>
       </c>
@@ -612,7 +612,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>30610</v>
       </c>
@@ -632,7 +632,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>30630</v>
       </c>
@@ -652,7 +652,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>30640</v>
       </c>
@@ -672,7 +672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>30650</v>
       </c>
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>30710</v>
       </c>
@@ -712,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>30680</v>
       </c>
@@ -732,7 +732,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>30690</v>
       </c>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>30700</v>
       </c>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>30720</v>
       </c>
@@ -792,7 +792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>30660</v>
       </c>
@@ -812,7 +812,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>30730</v>
       </c>
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>30740</v>
       </c>
@@ -852,7 +852,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>30750</v>
       </c>
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>30760</v>
       </c>
@@ -892,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>30770</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>30780</v>
       </c>
@@ -932,7 +932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>30790</v>
       </c>
@@ -952,7 +952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>30800</v>
       </c>
@@ -972,7 +972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>30810</v>
       </c>
@@ -992,7 +992,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>30820</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>30830</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>30850</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>30840</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>30860</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>30870</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>30880</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>30670</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30890</v>
       </c>

</xml_diff>

<commit_message>
Added system wise evalution in BHS calculator
</commit_message>
<xml_diff>
--- a/Biomarker_annotation.xlsx
+++ b/Biomarker_annotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catri\OneDrive\Documents\MSc HDA\Translational Data Sciences\BEES_TDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/lc5415_ic_ac_uk/Documents/MScHDA/Term2/TDS/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{9A24B856-B701-2743-ADFC-7E0A35D99268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7D89798-0B7E-4087-9888-7BB72877E340}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{9A24B856-B701-2743-ADFC-7E0A35D99268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93A52E37-E437-2B4D-A716-125C2672DB6F}"/>
   <bookViews>
-    <workbookView xWindow="10490" yWindow="0" windowWidth="7500" windowHeight="10200" xr2:uid="{85285DCB-5536-7D41-BDF8-0554B552EAE8}"/>
+    <workbookView xWindow="-25600" yWindow="5600" windowWidth="25600" windowHeight="16000" xr2:uid="{85285DCB-5536-7D41-BDF8-0554B552EAE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="44">
   <si>
     <t>Alanine aminotransferase</t>
   </si>
@@ -146,22 +146,25 @@
     <t>Liver</t>
   </si>
   <si>
-    <t>Liver Synthetic</t>
-  </si>
-  <si>
-    <t>System by paper</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>System by Fran</t>
-  </si>
-  <si>
-    <t>More_is_bad_Mantej</t>
-  </si>
-  <si>
-    <t>More_is_bad_paper</t>
+    <t>System.Paper</t>
+  </si>
+  <si>
+    <t>System.Barbara</t>
+  </si>
+  <si>
+    <t>MoreIsBad.Mantej</t>
+  </si>
+  <si>
+    <t>MoreIsBad.Paper</t>
+  </si>
+  <si>
+    <t>MoreIsBad.Barbara</t>
+  </si>
+  <si>
+    <t>System.Mantej</t>
   </si>
 </sst>
 </file>
@@ -536,23 +539,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06EC7B42-54D3-D849-9328-5C0F1D16A97A}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="2" customWidth="1"/>
     <col min="5" max="6" width="21.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="19.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -560,19 +565,25 @@
         <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>30620</v>
       </c>
@@ -585,14 +596,20 @@
       <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>30600</v>
       </c>
@@ -600,19 +617,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="2">
+        <v>37</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>30610</v>
       </c>
@@ -623,16 +646,22 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>30630</v>
       </c>
@@ -643,16 +672,22 @@
         <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>30640</v>
       </c>
@@ -663,16 +698,22 @@
         <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>30650</v>
       </c>
@@ -685,14 +726,20 @@
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2">
-        <v>1</v>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>30710</v>
       </c>
@@ -705,14 +752,20 @@
       <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="2">
-        <v>1</v>
+      <c r="E8" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>30680</v>
       </c>
@@ -723,16 +776,22 @@
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="2">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="2">
         <v>-1</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>30690</v>
       </c>
@@ -745,14 +804,20 @@
       <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
+      <c r="E10" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>30700</v>
       </c>
@@ -765,14 +830,20 @@
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2">
         <v>-1</v>
       </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>30720</v>
       </c>
@@ -783,16 +854,22 @@
         <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>30660</v>
       </c>
@@ -803,16 +880,22 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>30730</v>
       </c>
@@ -825,14 +908,20 @@
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="2">
-        <v>1</v>
+      <c r="E14" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>30740</v>
       </c>
@@ -843,16 +932,22 @@
         <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2">
         <v>-1</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>30750</v>
       </c>
@@ -865,14 +960,20 @@
       <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="2">
-        <v>1</v>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>30760</v>
       </c>
@@ -885,14 +986,20 @@
       <c r="D17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="2">
-        <v>0</v>
+      <c r="E17" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>30770</v>
       </c>
@@ -905,14 +1012,20 @@
       <c r="D18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="2">
         <v>-1</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>30780</v>
       </c>
@@ -923,16 +1036,22 @@
         <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>30790</v>
       </c>
@@ -943,16 +1062,22 @@
         <v>33</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>30800</v>
       </c>
@@ -963,16 +1088,22 @@
         <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="2">
+        <v>37</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="2">
         <v>-1</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>30810</v>
       </c>
@@ -983,16 +1114,22 @@
         <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="2">
+        <v>37</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="2">
         <v>-1</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>30820</v>
       </c>
@@ -1003,16 +1140,22 @@
         <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>30830</v>
       </c>
@@ -1023,16 +1166,22 @@
         <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="2">
+        <v>37</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="2">
         <v>-1</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>30850</v>
       </c>
@@ -1045,14 +1194,20 @@
       <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="2">
         <v>-1</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>30840</v>
       </c>
@@ -1063,16 +1218,22 @@
         <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>30860</v>
       </c>
@@ -1083,16 +1244,22 @@
         <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="2">
+        <v>37</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="2">
         <v>-1</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>30870</v>
       </c>
@@ -1105,14 +1272,20 @@
       <c r="D28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="2">
-        <v>1</v>
+      <c r="E28" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="F28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>30880</v>
       </c>
@@ -1123,16 +1296,22 @@
         <v>33</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>30670</v>
       </c>
@@ -1143,16 +1322,22 @@
         <v>35</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30890</v>
       </c>
@@ -1163,13 +1348,19 @@
         <v>32</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="2">
+        <v>37</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="2">
         <v>0</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>39</v>
+      <c r="G31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>